<commit_message>
demo.py for yale demo
</commit_message>
<xml_diff>
--- a/Demo/data/mq_metadata.xlsx
+++ b/Demo/data/mq_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/OneDrive/Elucidata/NA_Correction/Demo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/OneDrive/Elucidata/NA_Correction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1294,7 @@
         <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
@@ -1311,7 +1311,7 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
         <v>90</v>
@@ -1328,7 +1328,7 @@
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
@@ -1345,7 +1345,7 @@
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
         <v>90</v>
@@ -1362,7 +1362,7 @@
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>90</v>
@@ -1379,7 +1379,7 @@
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" t="s">
         <v>90</v>
@@ -1396,7 +1396,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
         <v>90</v>
@@ -1413,7 +1413,7 @@
         <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
         <v>90</v>

</xml_diff>